<commit_message>
Comentarios + eliminar htmls del proceso inicial
</commit_message>
<xml_diff>
--- a/radares_geolocalizacion.xlsx
+++ b/radares_geolocalizacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpino\OneDrive - CSI Ingenieros - CIEMSA\Escritorio\Automatizaciones\Radares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpino\OneDrive - CSI Ingenieros - CIEMSA\Escritorio\dev\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A635B5B-0B51-43EC-AA58-43ADE8F36079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8AD2D5-C060-46C3-99B9-8037BB747B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-975" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-975" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linea Base" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="235">
   <si>
     <t>Nombre de video</t>
   </si>
@@ -967,7 +967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1022,6 +1022,14 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4842,20 +4850,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A2CC30-B04A-4F4A-B9CB-C95B4F839A52}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C89" sqref="A89:C89"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5546875"/>
-    <col min="2" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4865,11 +4873,14 @@
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -4879,11 +4890,14 @@
       <c r="C2" s="10">
         <v>-56.002303599999998</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="44">
+        <v>200</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -4893,11 +4907,14 @@
       <c r="C3" s="9">
         <v>-55.998949600000003</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="45">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
@@ -4907,11 +4924,14 @@
       <c r="C4" s="9">
         <v>-55.954160999999999</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="45">
+        <v>200</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -4921,11 +4941,14 @@
       <c r="C5" s="9">
         <v>-55.873260000000002</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="45">
+        <v>200</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -4935,11 +4958,14 @@
       <c r="C6" s="9">
         <v>-55.871923099999997</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="45">
+        <v>200</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>38</v>
       </c>
@@ -4949,11 +4975,14 @@
       <c r="C7" s="17">
         <v>-55.857360800000002</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="45">
+        <v>200</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -4963,11 +4992,14 @@
       <c r="C8" s="9">
         <v>-55.823006800000002</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="45">
+        <v>200</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -4977,14 +5009,17 @@
       <c r="C9" s="9">
         <v>-55.821438499999999</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="45">
+        <v>200</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -4994,11 +5029,14 @@
       <c r="C10" s="9">
         <v>-56.703671800000002</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="45">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -5008,11 +5046,14 @@
       <c r="C11" s="10">
         <v>-57.259965800000003</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="44">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -5022,11 +5063,14 @@
       <c r="C12" s="9">
         <v>-57.815629999999999</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="45">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -5036,11 +5080,14 @@
       <c r="C13" s="10">
         <v>-57.0504927</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="44">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
@@ -5050,11 +5097,14 @@
       <c r="C14" s="9">
         <v>-57.059014400000002</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="45">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -5064,11 +5114,14 @@
       <c r="C15" s="10">
         <v>-56.0015517</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="44">
+        <v>101</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -5078,11 +5131,14 @@
       <c r="C16" s="9">
         <v>-56.003157100000003</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="44">
+        <v>101</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -5092,11 +5148,14 @@
       <c r="C17" s="9">
         <v>-56.021951199999997</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="45">
+        <v>8</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -5106,11 +5165,14 @@
       <c r="C18" s="10">
         <v>-56.008850700000004</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="44">
+        <v>8</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
@@ -5120,14 +5182,17 @@
       <c r="C19" s="9">
         <v>-57.583912499999997</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="45">
+        <v>3</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -5137,11 +5202,14 @@
       <c r="C20" s="9">
         <v>-53.8524654</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="45">
+        <v>9</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>66</v>
       </c>
@@ -5151,11 +5219,14 @@
       <c r="C21" s="9">
         <v>-53.4474619</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="45">
+        <v>9</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -5165,11 +5236,14 @@
       <c r="C22" s="10">
         <v>-56.624226200000003</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="44">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -5179,11 +5253,14 @@
       <c r="C23" s="9">
         <v>-56.262855600000002</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="45">
+        <v>5</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
@@ -5193,11 +5270,14 @@
       <c r="C24" s="9">
         <v>-57.040420599999997</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="45">
+        <v>11</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -5207,11 +5287,14 @@
       <c r="C25" s="10">
         <v>-55.578742900000002</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="44">
+        <v>200</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -5221,11 +5304,14 @@
       <c r="C26" s="10">
         <v>-56.800864300000001</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="44">
+        <v>11</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -5235,11 +5321,14 @@
       <c r="C27" s="9">
         <v>-57.092161300000001</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="45">
+        <v>23</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>77</v>
       </c>
@@ -5249,11 +5338,14 @@
       <c r="C28" s="9">
         <v>-56.4898831</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="45">
+        <v>30</v>
+      </c>
+      <c r="E28" s="14" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
@@ -5263,14 +5355,17 @@
       <c r="C29" s="9">
         <v>-56.458178099999998</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="45">
+        <v>30</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -5280,11 +5375,14 @@
       <c r="C30" s="9">
         <v>-56.807663599999998</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="45">
+        <v>11</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -5294,11 +5392,14 @@
       <c r="C31" s="9">
         <v>-56.4664675</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="45">
+        <v>30</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>24</v>
       </c>
@@ -5308,14 +5409,17 @@
       <c r="C32" s="20">
         <v>-58.202036999999997</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="46">
+        <v>21</v>
+      </c>
+      <c r="E32" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
@@ -5325,11 +5429,14 @@
       <c r="C33" s="9">
         <v>-56.509189399999997</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="45">
+        <v>5</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>71</v>
       </c>
@@ -5339,11 +5446,14 @@
       <c r="C34" s="9">
         <v>-56.498287699999999</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="45">
+        <v>5</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>72</v>
       </c>
@@ -5353,11 +5463,14 @@
       <c r="C35" s="9">
         <v>-55.975533300000002</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="45">
+        <v>5</v>
+      </c>
+      <c r="E35" s="14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>73</v>
       </c>
@@ -5367,11 +5480,14 @@
       <c r="C36" s="9">
         <v>-55.982280299999999</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="45">
+        <v>5</v>
+      </c>
+      <c r="E36" s="14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5381,11 +5497,14 @@
       <c r="C37" s="9">
         <v>-55.941409</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="45">
+        <v>5</v>
+      </c>
+      <c r="E37" s="14" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>74</v>
       </c>
@@ -5395,14 +5514,17 @@
       <c r="C38" s="20">
         <v>-55.938369799999997</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="46">
+        <v>5</v>
+      </c>
+      <c r="E38" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>62</v>
       </c>
@@ -5412,11 +5534,14 @@
       <c r="C39" s="9">
         <v>-54.152728400000001</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="45">
+        <v>7</v>
+      </c>
+      <c r="E39" s="14" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
@@ -5426,14 +5551,17 @@
       <c r="C40" s="9">
         <v>-54.168310200000001</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="45">
+        <v>8</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>61</v>
       </c>
@@ -5443,11 +5571,14 @@
       <c r="C41" s="9">
         <v>-54.212487899999999</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="45">
+        <v>26</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>
@@ -5457,11 +5588,14 @@
       <c r="C42" s="9">
         <v>-54.383471800000002</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="45">
+        <v>8</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>64</v>
       </c>
@@ -5471,11 +5605,14 @@
       <c r="C43" s="9">
         <v>-54.754349499999996</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="45">
+        <v>8</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>65</v>
       </c>
@@ -5485,11 +5622,14 @@
       <c r="C44" s="9">
         <v>-53.549693400000002</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="45">
+        <v>19</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>35</v>
       </c>
@@ -5499,11 +5639,14 @@
       <c r="C45" s="9">
         <v>-56.0241744</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="45">
+        <v>102</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
@@ -5513,11 +5656,14 @@
       <c r="C46" s="10">
         <v>-56.420951000000002</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="44">
+        <v>1</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -5527,11 +5673,14 @@
       <c r="C47" s="9">
         <v>-56.424495999999998</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="45">
+        <v>1</v>
+      </c>
+      <c r="E47" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>87</v>
       </c>
@@ -5541,11 +5690,14 @@
       <c r="C48" s="9">
         <v>-56.911199000000003</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="45">
+        <v>14</v>
+      </c>
+      <c r="E48" s="13" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>89</v>
       </c>
@@ -5555,11 +5707,14 @@
       <c r="C49" s="9">
         <v>-56.892353100000001</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="45">
+        <v>3</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>69</v>
       </c>
@@ -5569,11 +5724,14 @@
       <c r="C50" s="9">
         <v>-56.883106400000003</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="45">
+        <v>14</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>88</v>
       </c>
@@ -5583,11 +5741,14 @@
       <c r="C51" s="9">
         <v>-56.884320299999999</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="45">
+        <v>14</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>30</v>
       </c>
@@ -5597,14 +5758,17 @@
       <c r="C52" s="10">
         <v>-56.762297699999998</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="44">
+        <v>3</v>
+      </c>
+      <c r="E52" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>30</v>
       </c>
@@ -5614,11 +5778,14 @@
       <c r="C53" s="9">
         <v>-56.761255900000002</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="45">
+        <v>3</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>29</v>
       </c>
@@ -5628,11 +5795,14 @@
       <c r="C54" s="9">
         <v>-56.731166000000002</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="45">
+        <v>3</v>
+      </c>
+      <c r="E54" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>49</v>
       </c>
@@ -5642,11 +5812,14 @@
       <c r="C55" s="9">
         <v>-55.869084600000001</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="45">
+        <v>11</v>
+      </c>
+      <c r="E55" s="13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>49</v>
       </c>
@@ -5656,11 +5829,14 @@
       <c r="C56" s="9">
         <v>-55.876370799999997</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="45">
+        <v>11</v>
+      </c>
+      <c r="E56" s="14" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>10</v>
       </c>
@@ -5670,11 +5846,14 @@
       <c r="C57" s="10">
         <v>-56.377681500000001</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="44">
+        <v>11</v>
+      </c>
+      <c r="E57" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>8</v>
       </c>
@@ -5684,11 +5863,14 @@
       <c r="C58" s="9">
         <v>-56.298338299999998</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="45">
+        <v>11</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>42</v>
       </c>
@@ -5698,11 +5880,14 @@
       <c r="C59" s="9">
         <v>-56.233092399999997</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="45">
+        <v>1</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>50</v>
       </c>
@@ -5712,11 +5897,14 @@
       <c r="C60" s="9">
         <v>-55.767657</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="45">
+        <v>7</v>
+      </c>
+      <c r="E60" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>50</v>
       </c>
@@ -5726,11 +5914,14 @@
       <c r="C61" s="9">
         <v>-55.754062400000002</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="45">
+        <v>7</v>
+      </c>
+      <c r="E61" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
@@ -5740,14 +5931,17 @@
       <c r="C62" s="9">
         <v>-55.743663499999997</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="45">
+        <v>7</v>
+      </c>
+      <c r="E62" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>52</v>
       </c>
@@ -5757,11 +5951,14 @@
       <c r="C63" s="9">
         <v>-55.658239600000002</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="45">
+        <v>7</v>
+      </c>
+      <c r="E63" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
@@ -5771,11 +5968,14 @@
       <c r="C64" s="9">
         <v>-55.550547999999999</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="45">
+        <v>7</v>
+      </c>
+      <c r="E64" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>55</v>
       </c>
@@ -5785,11 +5985,14 @@
       <c r="C65" s="9">
         <v>-55.536468800000002</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" s="45">
+        <v>7</v>
+      </c>
+      <c r="E65" s="14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>43</v>
       </c>
@@ -5799,11 +6002,14 @@
       <c r="C66" s="9">
         <v>-56.204651900000002</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="E66" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>40</v>
       </c>
@@ -5813,11 +6019,14 @@
       <c r="C67" s="10">
         <v>-56.205157800000002</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="E67" s="13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>31</v>
       </c>
@@ -5827,11 +6036,14 @@
       <c r="C68" s="10">
         <v>-56.098802800000001</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="44">
+        <v>102</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>36</v>
       </c>
@@ -5841,11 +6053,14 @@
       <c r="C69" s="10">
         <v>-56.097112199999998</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="44">
+        <v>102</v>
+      </c>
+      <c r="E69" s="13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>43</v>
       </c>
@@ -5855,11 +6070,14 @@
       <c r="C70" s="10">
         <v>-56.151683599999998</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="44">
+        <v>102</v>
+      </c>
+      <c r="E70" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>45</v>
       </c>
@@ -5869,11 +6087,14 @@
       <c r="C71" s="9">
         <v>-56.245448799999998</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="45">
+        <v>102</v>
+      </c>
+      <c r="E71" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>56</v>
       </c>
@@ -5883,14 +6104,17 @@
       <c r="C72" s="9">
         <v>-55.152318700000002</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="D72" s="45">
+        <v>7</v>
+      </c>
+      <c r="E72" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>57</v>
       </c>
@@ -5900,11 +6124,14 @@
       <c r="C73" s="9">
         <v>-55.131984899999999</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" s="45">
+        <v>7</v>
+      </c>
+      <c r="E73" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>86</v>
       </c>
@@ -5914,11 +6141,14 @@
       <c r="C74" s="9">
         <v>-57.2092703</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D74" s="45">
+        <v>4</v>
+      </c>
+      <c r="E74" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>58</v>
       </c>
@@ -5928,11 +6158,14 @@
       <c r="C75" s="9">
         <v>-54.955321099999999</v>
       </c>
-      <c r="D75" s="14" t="s">
+      <c r="D75" s="45">
+        <v>7</v>
+      </c>
+      <c r="E75" s="14" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>58</v>
       </c>
@@ -5942,11 +6175,14 @@
       <c r="C76" s="9">
         <v>-54.929890100000001</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D76" s="45">
+        <v>7</v>
+      </c>
+      <c r="E76" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>59</v>
       </c>
@@ -5956,11 +6192,14 @@
       <c r="C77" s="9">
         <v>-54.765693200000001</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D77" s="45">
+        <v>7</v>
+      </c>
+      <c r="E77" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>60</v>
       </c>
@@ -5970,11 +6209,14 @@
       <c r="C78" s="9">
         <v>-54.541922999999997</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D78" s="45">
+        <v>7</v>
+      </c>
+      <c r="E78" s="14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>60</v>
       </c>
@@ -5984,11 +6226,14 @@
       <c r="C79" s="9">
         <v>-54.515222299999998</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="45">
+        <v>7</v>
+      </c>
+      <c r="E79" s="14" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>83</v>
       </c>
@@ -5998,11 +6243,14 @@
       <c r="C80" s="9">
         <v>-57.885954699999999</v>
       </c>
-      <c r="D80" s="13" t="s">
+      <c r="D80" s="45">
+        <v>3</v>
+      </c>
+      <c r="E80" s="13" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -6012,11 +6260,14 @@
       <c r="C81" s="9">
         <v>-57.904645799999997</v>
       </c>
-      <c r="D81" s="13" t="s">
+      <c r="D81" s="45">
+        <v>3</v>
+      </c>
+      <c r="E81" s="13" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
@@ -6026,14 +6277,17 @@
       <c r="C82" s="9">
         <v>-57.913722999999997</v>
       </c>
-      <c r="D82" s="13" t="s">
+      <c r="D82" s="45">
+        <v>3</v>
+      </c>
+      <c r="E82" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>79</v>
       </c>
@@ -6043,11 +6297,14 @@
       <c r="C83" s="9">
         <v>-57.9413318</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="45">
+        <v>3</v>
+      </c>
+      <c r="E83" s="14" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>22</v>
       </c>
@@ -6057,11 +6314,14 @@
       <c r="C84" s="9">
         <v>-57.837290299999999</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="45">
+        <v>21</v>
+      </c>
+      <c r="E84" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>23</v>
       </c>
@@ -6071,11 +6331,14 @@
       <c r="C85" s="9">
         <v>-57.8996998</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="45">
+        <v>55</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -6085,11 +6348,14 @@
       <c r="C86" s="10">
         <v>-58.288347700000003</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="44">
+        <v>21</v>
+      </c>
+      <c r="E86" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>9</v>
       </c>
@@ -6099,11 +6365,14 @@
       <c r="C87" s="9">
         <v>-56.282217600000003</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D87" s="45">
+        <v>81</v>
+      </c>
+      <c r="E87" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>15</v>
       </c>
@@ -6113,11 +6382,14 @@
       <c r="C88" s="10">
         <v>-56.068053300000003</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="44">
+        <v>107</v>
+      </c>
+      <c r="E88" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>6</v>
       </c>
@@ -6127,11 +6399,14 @@
       <c r="C89" s="9">
         <v>-56.201969499999997</v>
       </c>
-      <c r="D89" s="12" t="s">
+      <c r="D89" s="45">
+        <v>67</v>
+      </c>
+      <c r="E89" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="38" t="s">
         <v>6</v>
       </c>
@@ -6141,11 +6416,14 @@
       <c r="C90" s="40">
         <v>-56.204990500000001</v>
       </c>
-      <c r="D90" s="41" t="s">
+      <c r="D90" s="47">
+        <v>67</v>
+      </c>
+      <c r="E90" s="41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>13</v>
       </c>
@@ -6155,11 +6433,14 @@
       <c r="C91" s="10">
         <v>-56.070499099999999</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D91" s="44">
+        <v>107</v>
+      </c>
+      <c r="E91" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>36</v>
       </c>
@@ -6169,11 +6450,14 @@
       <c r="C92" s="9">
         <v>-56.019251300000001</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="45">
+        <v>74</v>
+      </c>
+      <c r="E92" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>11</v>
       </c>
@@ -6183,11 +6467,14 @@
       <c r="C93" s="9">
         <v>-56.051596600000003</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="45">
+        <v>74</v>
+      </c>
+      <c r="E93" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>48</v>
       </c>
@@ -6197,11 +6484,14 @@
       <c r="C94" s="10">
         <v>-55.968122999999999</v>
       </c>
-      <c r="D94" s="13" t="s">
+      <c r="D94" s="44">
+        <v>75</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>84</v>
       </c>
@@ -6211,11 +6501,14 @@
       <c r="C95" s="9">
         <v>-58.003717999999999</v>
       </c>
-      <c r="D95" s="13" t="s">
+      <c r="D95" s="45">
+        <v>3</v>
+      </c>
+      <c r="E95" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>82</v>
       </c>
@@ -6225,11 +6518,14 @@
       <c r="C96" s="9">
         <v>-57.8914878</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D96" s="45">
+        <v>3</v>
+      </c>
+      <c r="E96" s="13" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>85</v>
       </c>
@@ -6239,11 +6535,14 @@
       <c r="C97" s="9">
         <v>-58.045538200000003</v>
       </c>
-      <c r="D97" s="13" t="s">
+      <c r="D97" s="45">
+        <v>101</v>
+      </c>
+      <c r="E97" s="13" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>38</v>
       </c>
@@ -6253,11 +6552,14 @@
       <c r="C98" s="10">
         <v>-55.890081100000003</v>
       </c>
-      <c r="D98" s="13" t="s">
+      <c r="D98" s="44">
+        <v>101</v>
+      </c>
+      <c r="E98" s="13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>47</v>
       </c>
@@ -6267,28 +6569,34 @@
       <c r="C99" s="10">
         <v>-55.8873611</v>
       </c>
-      <c r="D99" s="13" t="s">
+      <c r="D99" s="44">
+        <v>101</v>
+      </c>
+      <c r="E99" s="13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="42"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="42"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
+      <c r="D102" s="42"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D102">
-    <sortCondition ref="D1:D102"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E102">
+    <sortCondition ref="E1:E102"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6298,7 +6606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D553DAC-10CF-4A0B-85B1-AAAC54261F65}">
   <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="C64" sqref="C64:C92"/>
     </sheetView>
   </sheetViews>

</xml_diff>